<commit_message>
20200531 add backup process in release procedure
</commit_message>
<xml_diff>
--- a/manual/Release/Program_Release.xlsx
+++ b/manual/Release/Program_Release.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esl01298shr\Philippines Project\クロージング\技術移転資料一式\manual\Release\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daime\OneDrive\デスクトップ\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C729988E-FFD8-48EE-B33B-90A0EF7C4005}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="-45" windowWidth="10575" windowHeight="6375" activeTab="1"/>
+    <workbookView xWindow="3045" yWindow="660" windowWidth="22890" windowHeight="15060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1.Release Procedure" sheetId="5" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="98">
   <si>
     <t>#stop the app servers</t>
   </si>
@@ -409,10 +410,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>7. After test , stop test server</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>(2) stop test server</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -454,13 +451,45 @@
   </si>
   <si>
     <t>TEMP_DIR="/home/(user)/temp_dev/upload"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>add 0530</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>7. access to the url  , and take backup before program upload</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(1) access the url</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    * you need special db password ( refer to password.xls)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(2) goto [Manage Database] and take backup for target db</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>8 .login by admin user in the target db , and install or update the  module</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(3) the db backup includes raw data , so need to keep it by encoding</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>9. After test , stop test server</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -664,6 +693,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -699,6 +745,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -874,7 +937,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -885,12 +948,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
@@ -916,7 +979,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="C12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
@@ -958,7 +1021,7 @@
     </row>
     <row r="22" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C22" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.15">
@@ -989,22 +1052,22 @@
     <row r="29" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="30" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.15">
       <c r="C31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.15">
       <c r="C32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1014,11 +1077,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1068,7 +1131,7 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.15">
       <c r="C12" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>38</v>
@@ -1126,7 +1189,7 @@
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.15">
       <c r="C26" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.15">
@@ -1226,58 +1289,95 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="C49" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B51" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="C52" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D53" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="C54" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B56" s="4" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B56" s="5"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A57" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C58" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C59" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B60" s="5"/>
+      <c r="C60" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C61" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A64" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B66" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C67" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="D68" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C69" s="4" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C57" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="D58" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C59" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B60" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <hyperlinks>
-    <hyperlink ref="B49" r:id="rId1" location="%E5%A4%89%E6%95%B0-var1-%E3%81%AE%E5%80%A4%E3%82%92%E8%A1%A8%E7%A4%BA%E3%81%99%E3%82%8B" display="https://shellscript.sunone.me/variable.html - %E5%A4%89%E6%95%B0-var1-%E3%81%AE%E5%80%A4%E3%82%92%E8%A1%A8%E7%A4%BA%E3%81%99%E3%82%8B"/>
+    <hyperlink ref="B49" r:id="rId1" location="%E5%A4%89%E6%95%B0-var1-%E3%81%AE%E5%80%A4%E3%82%92%E8%A1%A8%E7%A4%BA%E3%81%99%E3%82%8B" display="https://shellscript.sunone.me/variable.html - %E5%A4%89%E6%95%B0-var1-%E3%81%AE%E5%80%A4%E3%82%92%E8%A1%A8%E7%A4%BA%E3%81%99%E3%82%8B" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1285,11 +1385,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:M69"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76:G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1521,7 +1621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C49" s="3" t="s">
         <v>75</v>
       </c>
@@ -1529,12 +1629,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B52" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C54" s="4" t="s">
         <v>57</v>
       </c>
@@ -1542,7 +1642,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B56" s="4" t="s">
         <v>56</v>
       </c>
@@ -1550,22 +1650,22 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C57" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.15">
       <c r="D58" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C59" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C60" s="4" t="s">
         <v>52</v>
       </c>
@@ -1573,8 +1673,42 @@
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A62" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="C63" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="C64" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B65" s="5"/>
+      <c r="C65" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C66" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A69" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>